<commit_message>
merge sa trimiti email
</commit_message>
<xml_diff>
--- a/CreateAccountsTemplate.xlsx
+++ b/CreateAccountsTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\Desktop\Facultate\IOC35Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C5DAFE-7B43-48D9-8125-6145944F40B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1590362B-EAB2-45DF-8EA3-B7B76EE71996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8715" yWindow="4440" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -51,12 +51,6 @@
     <t>Baba</t>
   </si>
   <si>
-    <t>aba2@mail.com</t>
-  </si>
-  <si>
-    <t>aba3@mail.com</t>
-  </si>
-  <si>
     <t>student</t>
   </si>
   <si>
@@ -67,6 +61,12 @@
   </si>
   <si>
     <t>Tod</t>
+  </si>
+  <si>
+    <t>andrei@mail.com</t>
+  </si>
+  <si>
+    <t>olivia@mail.com</t>
   </si>
 </sst>
 </file>
@@ -398,7 +398,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,13 +442,13 @@
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E2">
         <v>123</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -456,19 +456,19 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="E3">
         <v>123</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>